<commit_message>
modified function and test
</commit_message>
<xml_diff>
--- a/test/テスト_read.xlsx
+++ b/test/テスト_read.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\xshimin\git_work\KubotaHA\TranscribeExcelData\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53996979-B87C-4D25-8FAD-985C793BB561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220FC62C-4761-4B1F-9532-3CA382DBECE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="9600" windowWidth="28770" windowHeight="17250" xr2:uid="{90AC207A-EF8E-49E0-BAC3-99B3184B1A4F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>カラム1</t>
     <phoneticPr fontId="1"/>
@@ -130,16 +130,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>data2-2</t>
-  </si>
-  <si>
-    <t>data2-3</t>
-  </si>
-  <si>
     <t>data2-4</t>
-  </si>
-  <si>
-    <t>data2-5</t>
   </si>
   <si>
     <t>data2-6</t>
@@ -186,18 +177,9 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>data3-2</t>
-  </si>
-  <si>
-    <t>data3-3</t>
-  </si>
-  <si>
     <t>data3-4</t>
   </si>
   <si>
-    <t>data3-5</t>
-  </si>
-  <si>
     <t>data3-6</t>
   </si>
   <si>
@@ -229,6 +211,18 @@
   </si>
   <si>
     <t>data1-6</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>data2,3-2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>data2,3-3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>data2,3-5</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -334,7 +328,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -364,6 +358,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -757,9 +757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6A32A39-1044-4546-9492-BA7EF3989C03}">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -815,7 +813,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
@@ -833,7 +831,7 @@
         <v>19</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>20</v>
@@ -865,105 +863,104 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
         <v>29</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" t="s">
         <v>30</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" t="s">
         <v>31</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
         <v>32</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I3" t="s">
         <v>33</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J3" t="s">
         <v>34</v>
       </c>
-      <c r="H3" t="s">
+      <c r="K3" t="s">
         <v>35</v>
       </c>
-      <c r="I3" t="s">
+      <c r="L3" t="s">
         <v>36</v>
       </c>
-      <c r="J3" t="s">
+      <c r="M3" t="s">
         <v>37</v>
       </c>
-      <c r="K3" t="s">
+      <c r="N3" t="s">
         <v>38</v>
       </c>
-      <c r="L3" t="s">
+      <c r="O3" t="s">
         <v>39</v>
       </c>
-      <c r="M3" t="s">
+      <c r="P3" t="s">
         <v>40</v>
-      </c>
-      <c r="N3" t="s">
-        <v>41</v>
-      </c>
-      <c r="O3" t="s">
-        <v>42</v>
-      </c>
-      <c r="P3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="10"/>
+      <c r="E4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="H4" t="s">
         <v>47</v>
       </c>
-      <c r="C4" t="s">
+      <c r="I4" t="s">
         <v>48</v>
       </c>
-      <c r="D4" t="s">
+      <c r="J4" t="s">
         <v>49</v>
       </c>
-      <c r="E4" t="s">
+      <c r="K4" t="s">
         <v>50</v>
       </c>
-      <c r="F4" t="s">
+      <c r="L4" t="s">
         <v>51</v>
       </c>
-      <c r="G4" t="s">
+      <c r="M4" t="s">
         <v>52</v>
       </c>
-      <c r="H4" t="s">
+      <c r="N4" t="s">
         <v>53</v>
       </c>
-      <c r="I4" t="s">
+      <c r="O4" t="s">
         <v>54</v>
       </c>
-      <c r="J4" t="s">
+      <c r="P4" t="s">
         <v>55</v>
-      </c>
-      <c r="K4" t="s">
-        <v>56</v>
-      </c>
-      <c r="L4" t="s">
-        <v>57</v>
-      </c>
-      <c r="M4" t="s">
-        <v>58</v>
-      </c>
-      <c r="N4" t="s">
-        <v>59</v>
-      </c>
-      <c r="O4" t="s">
-        <v>60</v>
-      </c>
-      <c r="P4" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="F3:F4"/>
+  </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>